<commit_message>
add test case results
</commit_message>
<xml_diff>
--- a/tests/analysis/clusters_annotation_tables/amiodarone_24_hr_extracellexclude_cluster1_table.xlsx
+++ b/tests/analysis/clusters_annotation_tables/amiodarone_24_hr_extracellexclude_cluster1_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loreal-my.sharepoint.com/personal/louison_fresnais_loreal_com/Documents/Documents/GitHub/MANA/tests/analysis/clusters_annotation_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FAB6B408337F30CCBC04E7FDC9EF069789704CC9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{452FFB75-766E-438D-8444-46467F344444}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_85EAB600558736BB84A4F0FDC9EF06978970CC47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EF324BA-53DA-4FDF-A939-A4A3F05B5DF1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,12 +265,12 @@
     <t>Hexadecanoyl-[acyl-carrier protein:malonyl-CoA C-acyltransferase(decarboxylating, oxoacyl- and enoyl-reducing and thioester-hydrolysing) Fatty acid biosynthesis EC:2.3.1.85</t>
   </si>
   <si>
+    <t>DOWN</t>
+  </si>
+  <si>
     <t>UP</t>
   </si>
   <si>
-    <t>DOWN</t>
-  </si>
-  <si>
     <t xml:space="preserve">acetyl-CoA(4-) + D-glucosamine 6-phosphate --&gt; N-acetyl-D-glucosamine 6-phosphate(2-) + coenzyme A(4-) + proton </t>
   </si>
   <si>
@@ -388,7 +388,7 @@
     <t>['FASN']</t>
   </si>
   <si>
-    <t>['SLC27A1', 'SLC27A4']</t>
+    <t>['SLC27A4', 'SLC27A1']</t>
   </si>
   <si>
     <t>['OLAH']</t>
@@ -397,7 +397,7 @@
     <t>['OLAH', 'FASN']</t>
   </si>
   <si>
-    <t>['ELOVL2', 'ELOVL5', 'FASN', 'ELOVL6']</t>
+    <t>['ELOVL5', 'ELOVL2', 'FASN', 'ELOVL6']</t>
   </si>
   <si>
     <t>Aminosugar metabolism</t>
@@ -421,19 +421,19 @@
     <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=FASN</t>
   </si>
   <si>
+    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=SLC27A4</t>
+  </si>
+  <si>
+    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=OLAH</t>
+  </si>
+  <si>
+    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=ELOVL5</t>
+  </si>
+  <si>
     <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=SLC27A1</t>
   </si>
   <si>
-    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=OLAH</t>
-  </si>
-  <si>
     <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=ELOVL2</t>
-  </si>
-  <si>
-    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=SLC27A4</t>
-  </si>
-  <si>
-    <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=ELOVL5</t>
   </si>
   <si>
     <t>https://www.genecards.org/cgi-bin/carddisp.pl?gene=ELOVL6</t>
@@ -856,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>